<commit_message>
Updated instructions for building QuickBot MOOC v2. Not finished with the instructions yet.
</commit_message>
<xml_diff>
--- a/robots/quickbot/mooc/v2/quickbot_mooc_v2_parts.xlsx
+++ b/robots/quickbot/mooc/v2/quickbot_mooc_v2_parts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="137">
   <si>
     <t>BeagleBone Black</t>
   </si>
@@ -375,9 +375,6 @@
     <t>10 pairs JST Plug Connector RC Lipo Battery Male/Female</t>
   </si>
   <si>
-    <t>Male Red Battery Connectors</t>
-  </si>
-  <si>
     <t>Anytime Tools 127 pc Heat Shrink Wire Wrap</t>
   </si>
   <si>
@@ -393,12 +390,6 @@
     <t>Crimping Tool: 0.1-1.0 mm² Capacity, 16-28 AWG</t>
   </si>
   <si>
-    <t>2-pin Female Larger JST Volt Reg Connector</t>
-  </si>
-  <si>
-    <t>3-pin Female JST IR Sensor Connector</t>
-  </si>
-  <si>
     <t>DC-DC LM2596 Converter Adjustable Step Down Regulator 1.2-35V</t>
   </si>
   <si>
@@ -427,6 +418,18 @@
   </si>
   <si>
     <t>Wheel Encoder</t>
+  </si>
+  <si>
+    <t>2-pin Female 2mm-pitch JST Volt Reg Connector</t>
+  </si>
+  <si>
+    <t>3-pin Female 2mm-pitch JST IR Sensor Connector</t>
+  </si>
+  <si>
+    <t>2-pin Female 0.1in-pitch JST Volt Reg Connector</t>
+  </si>
+  <si>
+    <t>2-pin Female Red JST Battery Connectors</t>
   </si>
 </sst>
 </file>
@@ -1303,8 +1306,8 @@
   </sheetPr>
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1322,7 +1325,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="28">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1720,7 +1723,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="B19" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>76</v>
@@ -2021,7 +2024,7 @@
         <v>114</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C31" s="9">
         <v>5</v>
@@ -2048,7 +2051,7 @@
         <v>104</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C32" s="9">
         <v>2</v>
@@ -2585,7 +2588,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C52" s="9">
         <v>2</v>
@@ -2632,7 +2635,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="B54" s="3" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>76</v>
@@ -2658,7 +2661,7 @@
         <v>117</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C55" s="9">
         <v>1</v>
@@ -2682,7 +2685,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>70</v>
@@ -2709,7 +2712,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>63</v>
@@ -2736,7 +2739,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>74</v>
@@ -2793,7 +2796,7 @@
         <v>19</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C60" s="9">
         <v>1</v>
@@ -2857,10 +2860,10 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C67" s="9">
         <v>1</v>
@@ -2881,7 +2884,7 @@
         <v>15</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C68" s="9">
         <v>1</v>
@@ -2902,7 +2905,7 @@
         <v>25</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C69" s="9">
         <v>1</v>
@@ -2923,7 +2926,7 @@
         <v>14</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C70" s="9">
         <v>1</v>
@@ -2944,7 +2947,7 @@
         <v>24</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C71" s="9">
         <v>1</v>
@@ -2962,10 +2965,10 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C72" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
Finished building section for QuickBot MOOC v2. Need to add programming section and running section.
</commit_message>
<xml_diff>
--- a/robots/quickbot/mooc/v2/quickbot_mooc_v2_parts.xlsx
+++ b/robots/quickbot/mooc/v2/quickbot_mooc_v2_parts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="142">
   <si>
     <t>BeagleBone Black</t>
   </si>
@@ -430,6 +430,21 @@
   </si>
   <si>
     <t>2-pin Female Red JST Battery Connectors</t>
+  </si>
+  <si>
+    <t>LCD Digital Ohm VOLT Meter AC DC Voltmeter Multimeter</t>
+  </si>
+  <si>
+    <t>Drill Bit 9/64"</t>
+  </si>
+  <si>
+    <t>Dremel</t>
+  </si>
+  <si>
+    <t>Bosch CO2136 Cobalt Jobber Length Drill Bit, 9/64-Inch</t>
+  </si>
+  <si>
+    <t>Dremel 7700-1/15 MultiPro 7.2-Volt Cordless Rotary Tool Kit</t>
   </si>
 </sst>
 </file>
@@ -582,7 +597,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="161">
+  <cellStyleXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -666,6 +681,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -811,7 +827,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="161">
+  <cellStyles count="162">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -931,6 +947,7 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1304,10 +1321,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1699,63 +1716,67 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
-        <v>89</v>
+        <v>11</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="C18" s="9">
-        <v>1</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>76</v>
+        <v>10</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+      <c r="E18" s="9">
+        <v>10</v>
       </c>
       <c r="F18" s="4">
-        <v>39.950000000000003</v>
+        <v>0.5</v>
       </c>
       <c r="G18" s="4">
         <f>C18*F18</f>
-        <v>39.950000000000003</v>
+        <v>5</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="B19" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="9">
-        <v>2</v>
-      </c>
-      <c r="E19" s="9">
-        <v>2</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>76</v>
+      <c r="A19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="4">
+        <v>7.95</v>
+      </c>
+      <c r="G19" s="4">
+        <f>C19*F19</f>
+        <v>7.95</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="B20" s="3" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>76</v>
       </c>
       <c r="D20" s="9">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E20" s="9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>76</v>
@@ -1769,16 +1790,16 @@
     </row>
     <row r="21" spans="1:9">
       <c r="B21" s="3" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>76</v>
       </c>
       <c r="D21" s="9">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E21" s="9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>76</v>
@@ -1791,57 +1812,71 @@
       </c>
     </row>
     <row r="22" spans="1:9">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="B22" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>76</v>
+        <v>0</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1</v>
       </c>
       <c r="D22" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="9">
-        <v>2</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>44.95</v>
+      </c>
+      <c r="G22" s="4">
+        <f>C22*F22</f>
+        <v>44.95</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:9">
+      <c r="A23" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="B23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>76</v>
+        <v>56</v>
+      </c>
+      <c r="C23" s="9">
+        <v>1</v>
       </c>
       <c r="D23" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="9">
-        <v>2</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>2.35</v>
+      </c>
+      <c r="G23" s="4">
+        <f>C23*F23</f>
+        <v>2.35</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C24" s="9">
         <v>1</v>
@@ -1853,23 +1888,22 @@
         <v>1</v>
       </c>
       <c r="F24" s="4">
-        <v>12.95</v>
+        <v>2.95</v>
       </c>
       <c r="G24" s="4">
         <f>C24*F24</f>
-        <v>12.95</v>
+        <v>2.95</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="12"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="3" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
@@ -1881,82 +1915,75 @@
         <v>1</v>
       </c>
       <c r="F25" s="4">
-        <v>1.95</v>
+        <v>5.95</v>
       </c>
       <c r="G25" s="4">
         <f>C25*F25</f>
-        <v>1.95</v>
+        <v>5.95</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="5"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
       </c>
-      <c r="D26" s="9">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9">
-        <v>1</v>
+      <c r="D26" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="F26" s="4">
-        <v>3.75</v>
+        <v>39.950000000000003</v>
       </c>
       <c r="G26" s="4">
         <f>C26*F26</f>
-        <v>3.75</v>
+        <v>39.950000000000003</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I26" s="5"/>
+        <v>88</v>
+      </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="9">
-        <v>1</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="4">
-        <v>11.95</v>
-      </c>
-      <c r="G27" s="4">
-        <f>C27*F27</f>
-        <v>11.95</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I27" s="5"/>
+      <c r="B27" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="9">
+        <v>2</v>
+      </c>
+      <c r="E27" s="9">
+        <v>2</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="28" spans="1:9">
       <c r="B28" s="3" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>76</v>
       </c>
       <c r="D28" s="9">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E28" s="9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>76</v>
@@ -1967,377 +1994,357 @@
       <c r="H28" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9">
       <c r="B29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="9">
+        <v>10</v>
+      </c>
+      <c r="E29" s="9">
+        <v>10</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="B30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="9">
+        <v>2</v>
+      </c>
+      <c r="E30" s="9">
+        <v>2</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="B31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="9">
+        <v>2</v>
+      </c>
+      <c r="E31" s="9">
+        <v>2</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="9">
+        <v>1</v>
+      </c>
+      <c r="D32" s="9">
+        <v>1</v>
+      </c>
+      <c r="E32" s="9">
+        <v>1</v>
+      </c>
+      <c r="F32" s="4">
+        <v>12.95</v>
+      </c>
+      <c r="G32" s="4">
+        <f>C32*F32</f>
+        <v>12.95</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="12"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1</v>
+      </c>
+      <c r="D33" s="9">
+        <v>1</v>
+      </c>
+      <c r="E33" s="9">
+        <v>1</v>
+      </c>
+      <c r="F33" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="G33" s="4">
+        <f>C33*F33</f>
+        <v>1.95</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1</v>
+      </c>
+      <c r="D34" s="9">
+        <v>1</v>
+      </c>
+      <c r="E34" s="9">
+        <v>1</v>
+      </c>
+      <c r="F34" s="4">
+        <v>3.75</v>
+      </c>
+      <c r="G34" s="4">
+        <f>C34*F34</f>
+        <v>3.75</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="4">
+        <v>11.95</v>
+      </c>
+      <c r="G35" s="4">
+        <f>C35*F35</f>
+        <v>11.95</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="B36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="9">
+        <v>25</v>
+      </c>
+      <c r="E36" s="9">
+        <v>6</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="B37" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="9">
+      <c r="C37" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="9">
         <v>25</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E37" s="9">
         <v>4</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="3" t="s">
+      <c r="F37" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C38" s="9">
         <v>5</v>
       </c>
-      <c r="D30" s="9">
-        <v>1</v>
-      </c>
-      <c r="E30" s="9">
+      <c r="D38" s="9">
+        <v>1</v>
+      </c>
+      <c r="E38" s="9">
         <v>5</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F38" s="11">
         <v>9.9499999999999993</v>
       </c>
-      <c r="G30" s="4">
-        <f t="shared" ref="G30:G45" si="0">C30*F30</f>
+      <c r="G38" s="4">
+        <f t="shared" ref="G38:G51" si="0">C38*F38</f>
         <v>49.75</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H38" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="3" t="s">
+    <row r="39" spans="1:9">
+      <c r="A39" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C39" s="9">
         <v>5</v>
       </c>
-      <c r="D31" s="9">
-        <v>1</v>
-      </c>
-      <c r="E31" s="9">
+      <c r="D39" s="9">
+        <v>1</v>
+      </c>
+      <c r="E39" s="9">
         <v>5</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F39" s="11">
         <v>1.25</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G39" s="4">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H39" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="3" t="s">
+    <row r="40" spans="1:9">
+      <c r="A40" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C40" s="9">
         <v>2</v>
       </c>
-      <c r="D32" s="9">
-        <v>1</v>
-      </c>
-      <c r="E32" s="9">
+      <c r="D40" s="9">
+        <v>1</v>
+      </c>
+      <c r="E40" s="9">
         <v>2</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F40" s="11">
         <v>0.75</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G40" s="4">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="H40" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="3" t="s">
+    <row r="41" spans="1:9">
+      <c r="A41" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="9">
-        <v>1</v>
-      </c>
-      <c r="D33" s="9">
-        <v>1</v>
-      </c>
-      <c r="E33" s="9">
-        <v>1</v>
-      </c>
-      <c r="F33" s="11">
+      <c r="C41" s="9">
+        <v>1</v>
+      </c>
+      <c r="D41" s="9">
+        <v>1</v>
+      </c>
+      <c r="E41" s="9">
+        <v>1</v>
+      </c>
+      <c r="F41" s="11">
         <v>0.75</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G41" s="4">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="H33" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" s="9">
-        <v>1</v>
-      </c>
-      <c r="D34" s="9">
-        <v>6</v>
-      </c>
-      <c r="E34" s="9">
-        <v>2</v>
-      </c>
-      <c r="F34" s="11">
-        <v>0.99</v>
-      </c>
-      <c r="G34" s="4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="9">
-        <v>1</v>
-      </c>
-      <c r="D35" s="9">
-        <v>50</v>
-      </c>
-      <c r="E35" s="9">
-        <v>18</v>
-      </c>
-      <c r="F35" s="4">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="G35" s="4">
-        <f t="shared" si="0"/>
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" s="9">
-        <v>1</v>
-      </c>
-      <c r="D36" s="9">
-        <v>100</v>
-      </c>
-      <c r="E36" s="9">
-        <v>61</v>
-      </c>
-      <c r="F36" s="4">
-        <v>7.95</v>
-      </c>
-      <c r="G36" s="4">
-        <f t="shared" si="0"/>
-        <v>7.95</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="9">
-        <v>1</v>
-      </c>
-      <c r="D37" s="9">
-        <v>25</v>
-      </c>
-      <c r="E37" s="9">
-        <v>17</v>
-      </c>
-      <c r="F37" s="4">
-        <v>0.59</v>
-      </c>
-      <c r="G37" s="4">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="9">
-        <v>1</v>
-      </c>
-      <c r="D38" s="9">
-        <v>25</v>
-      </c>
-      <c r="E38" s="9">
-        <v>18</v>
-      </c>
-      <c r="F38" s="4">
-        <v>0.69</v>
-      </c>
-      <c r="G38" s="4">
-        <f t="shared" si="0"/>
-        <v>0.69</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" s="9">
-        <v>1</v>
-      </c>
-      <c r="D39" s="9">
-        <v>25</v>
-      </c>
-      <c r="E39" s="9">
-        <v>1</v>
-      </c>
-      <c r="F39" s="4">
-        <v>0.79</v>
-      </c>
-      <c r="G39" s="4">
-        <f t="shared" si="0"/>
-        <v>0.79</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="9">
-        <v>1</v>
-      </c>
-      <c r="D40" s="9">
-        <v>10</v>
-      </c>
-      <c r="E40" s="9">
-        <v>1</v>
-      </c>
-      <c r="F40" s="4">
-        <v>0.69</v>
-      </c>
-      <c r="G40" s="4">
-        <f t="shared" si="0"/>
-        <v>0.69</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41" s="9">
-        <v>1</v>
-      </c>
-      <c r="D41" s="9">
-        <v>25</v>
-      </c>
-      <c r="E41" s="9">
-        <v>16</v>
-      </c>
-      <c r="F41" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="G41" s="4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
       <c r="H41" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>55</v>
+        <v>106</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C42" s="9">
         <v>1</v>
       </c>
       <c r="D42" s="9">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E42" s="9">
-        <v>10</v>
-      </c>
-      <c r="F42" s="4">
+        <v>2</v>
+      </c>
+      <c r="F42" s="11">
         <v>0.99</v>
       </c>
       <c r="G42" s="4">
@@ -2350,243 +2357,253 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="3" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C43" s="9">
         <v>1</v>
       </c>
       <c r="D43" s="9">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E43" s="9">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F43" s="4">
-        <v>0.99</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" si="0"/>
-        <v>0.99</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="H43" s="13" t="s">
         <v>92</v>
       </c>
+      <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="3" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C44" s="9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D44" s="9">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E44" s="9">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="F44" s="4">
-        <v>0.5</v>
+        <v>7.95</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7.95</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>30</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="3" t="s">
-        <v>90</v>
+        <v>98</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C45" s="9">
         <v>1</v>
       </c>
-      <c r="D45" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>76</v>
+      <c r="D45" s="9">
+        <v>25</v>
+      </c>
+      <c r="E45" s="9">
+        <v>17</v>
       </c>
       <c r="F45" s="4">
-        <v>7.95</v>
+        <v>0.59</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="0"/>
-        <v>7.95</v>
+        <v>0.59</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>30</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9">
+      <c r="A46" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="B46" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>76</v>
+        <v>85</v>
+      </c>
+      <c r="C46" s="9">
+        <v>1</v>
       </c>
       <c r="D46" s="9">
         <v>25</v>
       </c>
       <c r="E46" s="9">
-        <v>5</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>76</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="G46" s="4">
+        <f t="shared" si="0"/>
+        <v>0.69</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9">
+      <c r="A47" s="20" t="s">
+        <v>100</v>
+      </c>
       <c r="B47" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>76</v>
+        <v>86</v>
+      </c>
+      <c r="C47" s="9">
+        <v>1</v>
       </c>
       <c r="D47" s="9">
         <v>25</v>
       </c>
       <c r="E47" s="9">
-        <v>5</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="G47" s="4">
+        <f t="shared" si="0"/>
+        <v>0.79</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="3" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="C48" s="9">
         <v>1</v>
       </c>
       <c r="D48" s="9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E48" s="9">
         <v>1</v>
       </c>
       <c r="F48" s="4">
-        <v>44.95</v>
+        <v>0.69</v>
       </c>
       <c r="G48" s="4">
-        <f>C48*F48</f>
-        <v>44.95</v>
+        <f t="shared" si="0"/>
+        <v>0.69</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>92</v>
+      </c>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="3" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C49" s="9">
         <v>1</v>
       </c>
       <c r="D49" s="9">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E49" s="9">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F49" s="4">
-        <v>2.35</v>
+        <v>0.99</v>
       </c>
       <c r="G49" s="4">
-        <f>C49*F49</f>
-        <v>2.35</v>
+        <f t="shared" si="0"/>
+        <v>0.99</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>57</v>
+        <v>109</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="C50" s="9">
         <v>1</v>
       </c>
       <c r="D50" s="9">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E50" s="9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" s="4">
-        <v>2.95</v>
+        <v>0.99</v>
       </c>
       <c r="G50" s="4">
-        <f>C50*F50</f>
-        <v>2.95</v>
+        <f t="shared" si="0"/>
+        <v>0.99</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="C51" s="9">
         <v>1</v>
       </c>
       <c r="D51" s="9">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E51" s="9">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F51" s="4">
-        <v>5.95</v>
+        <v>0.99</v>
       </c>
       <c r="G51" s="4">
-        <f>C51*F51</f>
-        <v>5.95</v>
+        <f t="shared" si="0"/>
+        <v>0.99</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="3" t="s">
         <v>123</v>
       </c>
@@ -2610,7 +2627,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:8">
       <c r="B53" s="3" t="s">
         <v>66</v>
       </c>
@@ -2633,7 +2650,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:8">
       <c r="B54" s="3" t="s">
         <v>135</v>
       </c>
@@ -2656,7 +2673,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:8">
       <c r="A55" s="3" t="s">
         <v>117</v>
       </c>
@@ -2683,7 +2700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:8">
       <c r="A56" s="3" t="s">
         <v>118</v>
       </c>
@@ -2710,7 +2727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:8">
       <c r="A57" s="3" t="s">
         <v>119</v>
       </c>
@@ -2737,7 +2754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:8">
       <c r="A58" s="3" t="s">
         <v>120</v>
       </c>
@@ -2764,7 +2781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:8">
       <c r="A59" s="3" t="s">
         <v>39</v>
       </c>
@@ -2791,7 +2808,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:8">
       <c r="A60" s="3" t="s">
         <v>19</v>
       </c>
@@ -2818,7 +2835,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="6" customFormat="1" ht="20">
+    <row r="63" spans="1:8" s="6" customFormat="1" ht="20">
       <c r="A63" s="6" t="s">
         <v>17</v>
       </c>
@@ -2834,11 +2851,11 @@
       <c r="F63" s="7"/>
       <c r="G63" s="7">
         <f>SUM(G5:G62)</f>
-        <v>278.10999999999996</v>
+        <v>278.11</v>
       </c>
       <c r="H63" s="7"/>
     </row>
-    <row r="64" spans="1:9" s="22" customFormat="1" ht="20">
+    <row r="64" spans="1:8" s="22" customFormat="1" ht="20">
       <c r="C64" s="23"/>
       <c r="D64" s="23"/>
       <c r="E64" s="23"/>
@@ -2846,7 +2863,7 @@
       <c r="G64" s="24"/>
       <c r="H64" s="24"/>
     </row>
-    <row r="65" spans="1:9" s="25" customFormat="1" ht="20">
+    <row r="65" spans="1:8" s="25" customFormat="1" ht="20">
       <c r="A65" s="17" t="s">
         <v>28</v>
       </c>
@@ -2858,7 +2875,7 @@
       <c r="G65" s="27"/>
       <c r="H65" s="27"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:8">
       <c r="A67" s="3" t="s">
         <v>122</v>
       </c>
@@ -2879,7 +2896,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:8">
       <c r="A68" s="3" t="s">
         <v>15</v>
       </c>
@@ -2893,14 +2910,14 @@
         <v>4</v>
       </c>
       <c r="G68" s="4">
-        <f t="shared" ref="G68:G72" si="2">C68*F68</f>
+        <f t="shared" ref="G68:G75" si="2">C68*F68</f>
         <v>4</v>
       </c>
       <c r="H68" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:8">
       <c r="A69" s="3" t="s">
         <v>25</v>
       </c>
@@ -2921,7 +2938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:8">
       <c r="A70" s="3" t="s">
         <v>14</v>
       </c>
@@ -2942,7 +2959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:8">
       <c r="A71" s="3" t="s">
         <v>24</v>
       </c>
@@ -2963,7 +2980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:8">
       <c r="A72" s="3" t="s">
         <v>131</v>
       </c>
@@ -2984,204 +3001,267 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:9" s="6" customFormat="1" ht="20">
-      <c r="A74" s="6" t="s">
+    <row r="73" spans="1:8">
+      <c r="A73" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="9">
+        <v>1</v>
+      </c>
+      <c r="F73" s="4">
+        <v>8.81</v>
+      </c>
+      <c r="G73" s="4">
+        <f t="shared" si="2"/>
+        <v>8.81</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C74" s="9">
+        <v>1</v>
+      </c>
+      <c r="F74" s="4">
+        <v>2.97</v>
+      </c>
+      <c r="G74" s="4">
+        <f t="shared" si="2"/>
+        <v>2.97</v>
+      </c>
+      <c r="H74" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75" s="9">
+        <v>1</v>
+      </c>
+      <c r="F75" s="4">
+        <v>41.04</v>
+      </c>
+      <c r="G75" s="4">
+        <f t="shared" si="2"/>
+        <v>41.04</v>
+      </c>
+      <c r="H75" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="6" customFormat="1" ht="20">
+      <c r="A77" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C74" s="10">
+      <c r="C77" s="10">
         <f>SUM(C68:C71)</f>
         <v>4</v>
       </c>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7">
-        <f>SUMPRODUCT(C67:C73,G67:G73)</f>
-        <v>78.430000000000007</v>
-      </c>
-      <c r="H74" s="7"/>
-    </row>
-    <row r="75" spans="1:9" s="22" customFormat="1" ht="20">
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="24"/>
-      <c r="H75" s="24"/>
-    </row>
-    <row r="76" spans="1:9" s="25" customFormat="1" ht="20">
-      <c r="A76" s="17" t="s">
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7">
+        <f>SUMPRODUCT(C67:C76,G67:G76)</f>
+        <v>131.25</v>
+      </c>
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="1:8" s="22" customFormat="1" ht="20">
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+    </row>
+    <row r="79" spans="1:8" s="25" customFormat="1" ht="20">
+      <c r="A79" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B76" s="17"/>
-      <c r="C76" s="26"/>
-      <c r="D76" s="26"/>
-      <c r="E76" s="26"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="27"/>
-      <c r="H76" s="27"/>
-    </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="3" t="s">
+      <c r="B79" s="17"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="27"/>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C78" s="9">
-        <v>1</v>
-      </c>
-      <c r="F78" s="4">
+      <c r="C81" s="9">
+        <v>1</v>
+      </c>
+      <c r="F81" s="4">
         <v>6.5</v>
       </c>
-      <c r="G78" s="4">
-        <f>C78*F78</f>
+      <c r="G81" s="4">
+        <f>C81*F81</f>
         <v>6.5</v>
       </c>
-      <c r="H78" s="13" t="s">
+      <c r="H81" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I78" s="5" t="s">
+      <c r="I81" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="3" t="s">
+    <row r="82" spans="1:9">
+      <c r="A82" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C79" s="9">
-        <v>1</v>
-      </c>
-      <c r="F79" s="4">
+      <c r="C82" s="9">
+        <v>1</v>
+      </c>
+      <c r="F82" s="4">
         <v>5.95</v>
       </c>
-      <c r="G79" s="4">
-        <f t="shared" ref="G79:G84" si="3">C79*F79</f>
+      <c r="G82" s="4">
+        <f t="shared" ref="G82:G87" si="3">C82*F82</f>
         <v>5.95</v>
       </c>
-      <c r="H79" s="13" t="s">
+      <c r="H82" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I79" s="5" t="s">
+      <c r="I82" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="3" t="s">
+    <row r="83" spans="1:9">
+      <c r="A83" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="9">
-        <v>1</v>
-      </c>
-      <c r="F80" s="4">
+      <c r="C83" s="9">
+        <v>1</v>
+      </c>
+      <c r="F83" s="4">
         <v>6.95</v>
       </c>
-      <c r="G80" s="4">
+      <c r="G83" s="4">
         <f t="shared" si="3"/>
         <v>6.95</v>
       </c>
-      <c r="H80" s="13" t="s">
+      <c r="H83" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I80" s="5" t="s">
+      <c r="I83" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="3" t="s">
+    <row r="84" spans="1:9">
+      <c r="A84" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C81" s="9">
-        <v>1</v>
-      </c>
-      <c r="F81" s="4">
+      <c r="C84" s="9">
+        <v>1</v>
+      </c>
+      <c r="F84" s="4">
         <v>1.55</v>
       </c>
-      <c r="G81" s="4">
+      <c r="G84" s="4">
         <f t="shared" si="3"/>
         <v>1.55</v>
       </c>
-      <c r="H81" s="13" t="s">
+      <c r="H84" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="3" t="s">
+    <row r="85" spans="1:9">
+      <c r="A85" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C82" s="9">
-        <v>1</v>
-      </c>
-      <c r="F82" s="4">
+      <c r="C85" s="9">
+        <v>1</v>
+      </c>
+      <c r="F85" s="4">
         <v>0.76</v>
       </c>
-      <c r="G82" s="4">
+      <c r="G85" s="4">
         <f t="shared" si="3"/>
         <v>0.76</v>
       </c>
-      <c r="H82" s="13" t="s">
+      <c r="H85" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I82" s="5" t="s">
+      <c r="I85" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="3" t="s">
+    <row r="86" spans="1:9">
+      <c r="A86" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C83" s="9">
-        <v>1</v>
-      </c>
-      <c r="F83" s="4">
+      <c r="C86" s="9">
+        <v>1</v>
+      </c>
+      <c r="F86" s="4">
         <v>1.46</v>
       </c>
-      <c r="G83" s="4">
+      <c r="G86" s="4">
         <f t="shared" si="3"/>
         <v>1.46</v>
       </c>
-      <c r="H83" s="13" t="s">
+      <c r="H86" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="3" t="s">
+    <row r="87" spans="1:9">
+      <c r="A87" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C84" s="9">
-        <v>1</v>
-      </c>
-      <c r="F84" s="4">
+      <c r="C87" s="9">
+        <v>1</v>
+      </c>
+      <c r="F87" s="4">
         <v>11.46</v>
       </c>
-      <c r="G84" s="4">
+      <c r="G87" s="4">
         <f t="shared" si="3"/>
         <v>11.46</v>
       </c>
-      <c r="H84" s="13" t="s">
+      <c r="H87" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:9" s="6" customFormat="1" ht="20">
-      <c r="A86" s="6" t="s">
+    <row r="89" spans="1:9" s="6" customFormat="1" ht="20">
+      <c r="A89" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C86" s="10">
-        <f>SUM(C78:C85)</f>
+      <c r="C89" s="10">
+        <f>SUM(C81:C88)</f>
         <v>7</v>
       </c>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7">
-        <f>SUMPRODUCT(C78:C85,G78:G85)</f>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7">
+        <f>SUMPRODUCT(C81:C88,G81:G88)</f>
         <v>34.630000000000003</v>
       </c>
-      <c r="H86" s="7"/>
+      <c r="H89" s="7"/>
     </row>
   </sheetData>
   <sortState ref="A50:S52">
     <sortCondition ref="K50:K52"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>
-  <conditionalFormatting sqref="M78:XFD79 C24 F24 M40:XFD43 A24:B28 M24:XFD28 H35:I35 C27 F27 H24:I27 I40:I43 A48:B49 M48:XFD49 H48:I49 D28:E34 C52 D53:E53 F52 H50:H52 I28 C54:E54 H55:H57 I36:I38 M35:XFD38 A35:B43 H36:H44 C25:F26 C48:F51 C55:F59 C35:F44 A78:F79 H78:H79">
+  <conditionalFormatting sqref="M81:XFD82 C32 F32 M48:XFD51 A32:B36 M32:XFD36 H43:I43 C35 F35 H32:I35 I48:I51 A22:B23 M22:XFD23 H22:I23 D36:E42 C52 D53:E53 F52 I36 C54:E54 H55:H57 I44:I46 M43:XFD46 C33:F34 C22:F25 C55:F59 A81:F82 H81:H82 H24:H25 H44:H52 H18 A43:F51 C18:F18">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="formula" val="MOD(ROW(),2)=1"/>
@@ -3201,7 +3281,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H30:H34">
+  <conditionalFormatting sqref="H38:H42">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="MOD(ROW(),2)=1"/>
@@ -3222,49 +3302,49 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I48" r:id="rId1"/>
-    <hyperlink ref="I49" r:id="rId2"/>
-    <hyperlink ref="I78" r:id="rId3"/>
-    <hyperlink ref="I79" r:id="rId4"/>
-    <hyperlink ref="I80" r:id="rId5"/>
-    <hyperlink ref="I82" r:id="rId6"/>
-    <hyperlink ref="H24" r:id="rId7"/>
-    <hyperlink ref="H48" r:id="rId8" display="SparkFun  "/>
-    <hyperlink ref="H25" r:id="rId9"/>
-    <hyperlink ref="H44" r:id="rId10"/>
+    <hyperlink ref="I22" r:id="rId1"/>
+    <hyperlink ref="I23" r:id="rId2"/>
+    <hyperlink ref="I81" r:id="rId3"/>
+    <hyperlink ref="I82" r:id="rId4"/>
+    <hyperlink ref="I83" r:id="rId5"/>
+    <hyperlink ref="I85" r:id="rId6"/>
+    <hyperlink ref="H32" r:id="rId7"/>
+    <hyperlink ref="H22" r:id="rId8" display="SparkFun  "/>
+    <hyperlink ref="H33" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId10"/>
     <hyperlink ref="H68" r:id="rId11"/>
     <hyperlink ref="H69" r:id="rId12"/>
     <hyperlink ref="H70" r:id="rId13"/>
     <hyperlink ref="H71" r:id="rId14"/>
-    <hyperlink ref="H78" r:id="rId15"/>
-    <hyperlink ref="H79" r:id="rId16"/>
-    <hyperlink ref="H80" r:id="rId17"/>
-    <hyperlink ref="H81" r:id="rId18"/>
-    <hyperlink ref="H82" r:id="rId19"/>
-    <hyperlink ref="H83" r:id="rId20"/>
-    <hyperlink ref="H84" r:id="rId21"/>
+    <hyperlink ref="H81" r:id="rId15"/>
+    <hyperlink ref="H82" r:id="rId16"/>
+    <hyperlink ref="H83" r:id="rId17"/>
+    <hyperlink ref="H84" r:id="rId18"/>
+    <hyperlink ref="H85" r:id="rId19"/>
+    <hyperlink ref="H86" r:id="rId20"/>
+    <hyperlink ref="H87" r:id="rId21"/>
     <hyperlink ref="H5" r:id="rId22" display="SparkFun  "/>
-    <hyperlink ref="H18" r:id="rId23"/>
-    <hyperlink ref="H45" r:id="rId24" display="SparkFun (Resistor Kit - 1/4W)"/>
-    <hyperlink ref="H26" r:id="rId25"/>
-    <hyperlink ref="H35" r:id="rId26"/>
-    <hyperlink ref="H37" r:id="rId27"/>
-    <hyperlink ref="H38" r:id="rId28"/>
-    <hyperlink ref="H39" r:id="rId29"/>
-    <hyperlink ref="H40" r:id="rId30"/>
-    <hyperlink ref="H36" r:id="rId31"/>
-    <hyperlink ref="H27" r:id="rId32"/>
-    <hyperlink ref="H30" r:id="rId33"/>
-    <hyperlink ref="H32" r:id="rId34"/>
-    <hyperlink ref="H33" r:id="rId35"/>
-    <hyperlink ref="H34" r:id="rId36"/>
-    <hyperlink ref="H41" r:id="rId37"/>
-    <hyperlink ref="H42" r:id="rId38"/>
-    <hyperlink ref="H43" r:id="rId39"/>
-    <hyperlink ref="H49" r:id="rId40"/>
-    <hyperlink ref="H50" r:id="rId41"/>
-    <hyperlink ref="H31" r:id="rId42"/>
-    <hyperlink ref="H51" r:id="rId43"/>
+    <hyperlink ref="H26" r:id="rId23"/>
+    <hyperlink ref="H19" r:id="rId24" display="SparkFun (Resistor Kit - 1/4W)"/>
+    <hyperlink ref="H34" r:id="rId25"/>
+    <hyperlink ref="H43" r:id="rId26"/>
+    <hyperlink ref="H45" r:id="rId27"/>
+    <hyperlink ref="H46" r:id="rId28"/>
+    <hyperlink ref="H47" r:id="rId29"/>
+    <hyperlink ref="H48" r:id="rId30"/>
+    <hyperlink ref="H44" r:id="rId31"/>
+    <hyperlink ref="H35" r:id="rId32"/>
+    <hyperlink ref="H38" r:id="rId33"/>
+    <hyperlink ref="H40" r:id="rId34"/>
+    <hyperlink ref="H41" r:id="rId35"/>
+    <hyperlink ref="H42" r:id="rId36"/>
+    <hyperlink ref="H49" r:id="rId37"/>
+    <hyperlink ref="H50" r:id="rId38"/>
+    <hyperlink ref="H51" r:id="rId39"/>
+    <hyperlink ref="H23" r:id="rId40"/>
+    <hyperlink ref="H24" r:id="rId41"/>
+    <hyperlink ref="H39" r:id="rId42"/>
+    <hyperlink ref="H25" r:id="rId43"/>
     <hyperlink ref="H52" r:id="rId44"/>
     <hyperlink ref="H55" r:id="rId45"/>
     <hyperlink ref="H56" r:id="rId46"/>
@@ -3274,6 +3354,9 @@
     <hyperlink ref="H60" r:id="rId50"/>
     <hyperlink ref="H67" r:id="rId51"/>
     <hyperlink ref="H72" r:id="rId52"/>
+    <hyperlink ref="H73" r:id="rId53"/>
+    <hyperlink ref="H75" r:id="rId54"/>
+    <hyperlink ref="H74" r:id="rId55"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0" footer="0"/>

</xml_diff>